<commit_message>
entrega final - script
</commit_message>
<xml_diff>
--- a/scripts/ListaMacrofitasTests.xlsx
+++ b/scripts/ListaMacrofitasTests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="925" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="livros e artigos para tese" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,12 +15,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Dicliptera ciliaris Juss.</t>
   </si>
   <si>
-    <t>Justia pectoralis Jacq.</t>
+    <t>Panicum pernambuncense (Spreng.) Mez ex Pilg.</t>
+  </si>
+  <si>
+    <t>Reimarochloa acuta (Flüggé) Hitchc.</t>
+  </si>
+  <si>
+    <t>Sacciolepis myuros (Lam.) Chase</t>
+  </si>
+  <si>
+    <t>Urochloa plantaginea (Link) R. D. Webster</t>
   </si>
 </sst>
 </file>
@@ -125,7 +134,7 @@
   <dimension ref="A1:A924"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -143,6 +152,21 @@
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>